<commit_message>
Splitting Single Line and Multi-line
</commit_message>
<xml_diff>
--- a/Project/Staffing Optimization 24-Hour Ops Model - Linear Programming/data/demand.xlsx
+++ b/Project/Staffing Optimization 24-Hour Ops Model - Linear Programming/data/demand.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a459e8a3726ef50c/Documents/Code-Portofolio/Project/24-hr Fast Food Shift Schedule - Linear Programming/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a459e8a3726ef50c/Documents/Code-Portofolio/Project/Staffing Optimization 24-Hour Ops Model - Linear Programming/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_F25DC773A252ABDACC104851D1DF71E45BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEF82AB7-C127-44DF-9129-9256559EDCF3}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_F25DC773A252ABDACC104851D1DF71E45BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE10568B-EFBD-41E4-8A13-922D19987EC7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Period</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Service Req</t>
+  </si>
+  <si>
+    <t>Staff Req</t>
   </si>
 </sst>
 </file>
@@ -470,21 +473,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="24.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -501,13 +504,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -523,14 +529,18 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
+        <f>G2+H2</f>
+        <v>12</v>
+      </c>
+      <c r="G2" s="1">
         <v>8</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -546,14 +556,18 @@
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
+        <f>G3+H3</f>
+        <v>20</v>
+      </c>
+      <c r="G3" s="1">
         <v>14</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -569,14 +583,18 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
+        <f>G4+H4</f>
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
         <v>6</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -592,14 +610,18 @@
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
+        <f>G5+H5</f>
+        <v>18</v>
+      </c>
+      <c r="G5" s="1">
         <v>14</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -615,14 +637,18 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
+        <f>G6+H6</f>
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
         <v>7</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -638,10 +664,14 @@
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
+        <f>G7+H7</f>
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
         <v>4</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>